<commit_message>
Solved downwash interference I think
</commit_message>
<xml_diff>
--- a/Corrections/TailOffData.xlsx
+++ b/Corrections/TailOffData.xlsx
@@ -1,31 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tomassinnige\My Documents\surfdrive\LR TT\EDUCATION\AE4115\2020_2021\LAB EXERCISE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\PycharmProjects\experimental-simulations\Corrections\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA73A3A-43ED-4B6B-9145-A68A18D36C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AoS = 0 deg" sheetId="1" r:id="rId1"/>
     <sheet name="AoS variations" sheetId="2" r:id="rId2"/>
+    <sheet name="Extrapolation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>AoA</t>
   </si>
@@ -44,13 +57,16 @@
   <si>
     <t>CM25c</t>
   </si>
+  <si>
+    <t>Cldif</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -98,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -115,12 +131,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,7 +161,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -678,10 +698,10 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
-            <c:v>ReMAC=550k</c:v>
+            <c:v>ReMAC = 110k</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -695,11 +715,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -707,12 +727,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AoS = 0 deg'!$A$62:$A$72</c:f>
+              <c:f>'AoS = 0 deg'!$A$84:$A$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-4.9980000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4</c:v>
@@ -743,48 +763,102 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'AoS = 0 deg'!$D$62:$D$72</c:f>
+              <c:f>'AoS = 0 deg'!$D$84:$D$103</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>00,000</c:formatCode>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-0.17979999999999999</c:v>
+                  <c:v>-0.13570000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.5099999999999995E-2</c:v>
+                  <c:v>-4.7600000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1900000000000001E-2</c:v>
+                  <c:v>4.3200000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10879999999999999</c:v>
+                  <c:v>0.1331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20480000000000001</c:v>
+                  <c:v>0.2248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29970000000000002</c:v>
+                  <c:v>0.31779999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39279999999999998</c:v>
+                  <c:v>0.40689999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48470000000000002</c:v>
+                  <c:v>0.49869999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.57440000000000002</c:v>
+                  <c:v>0.58809999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66110000000000002</c:v>
+                  <c:v>0.6764</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74490000000000001</c:v>
+                  <c:v>0.76359999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.84540000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92230000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0247999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0547</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0681</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1087</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1218999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1689000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -792,7 +866,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-87F2-49C7-8162-10A4E0D803D7}"/>
+              <c16:uniqueId val="{00000001-C699-4139-8369-7B74FF663756}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -806,6 +880,143 @@
         </c:dLbls>
         <c:axId val="516330528"/>
         <c:axId val="516331184"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>ReMAC=550k</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'AoS = 0 deg'!$A$62:$A$72</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'AoS = 0 deg'!$D$62:$D$72</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0000</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>-0.17979999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-8.5099999999999995E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.1900000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.10879999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.20480000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.29970000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.39279999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.48470000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.57440000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.66110000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.74490000000000001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-87F2-49C7-8162-10A4E0D803D7}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="516330528"/>
@@ -854,7 +1065,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -880,7 +1090,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -918,7 +1128,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516331184"/>
@@ -972,7 +1182,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -998,7 +1207,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1036,7 +1245,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516330528"/>
@@ -1053,7 +1262,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1079,7 +1287,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1109,7 +1317,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1123,7 +1331,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1836,7 +2044,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1862,7 +2069,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1900,7 +2107,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516331184"/>
@@ -1954,7 +2161,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1980,7 +2186,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2018,7 +2224,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516330528"/>
@@ -2035,7 +2241,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2061,7 +2266,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2091,7 +2296,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2105,7 +2310,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2818,7 +3023,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2844,7 +3048,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2882,7 +3086,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516331184"/>
@@ -2941,7 +3145,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2967,7 +3170,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3005,7 +3208,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516330528"/>
@@ -3022,7 +3225,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3048,7 +3250,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3078,7 +3280,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3092,7 +3294,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3459,7 +3661,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3485,7 +3686,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3523,7 +3724,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516331184"/>
@@ -3577,7 +3778,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3603,7 +3803,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3641,7 +3841,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516330528"/>
@@ -3658,7 +3858,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3684,7 +3883,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3714,7 +3913,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3728,7 +3927,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4095,7 +4294,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4121,7 +4319,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4159,7 +4357,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516331184"/>
@@ -4213,7 +4411,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4239,7 +4436,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4277,7 +4474,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516330528"/>
@@ -4294,7 +4491,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4320,7 +4516,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4350,7 +4546,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4364,7 +4560,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4731,7 +4927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4757,7 +4952,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4795,7 +4990,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516331184"/>
@@ -4854,7 +5049,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4880,7 +5074,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4918,7 +5112,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="516330528"/>
@@ -4935,7 +5129,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4961,7 +5154,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4991,7 +5184,318 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Extrapolation!$H$1:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Extrapolation!$I$1:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-1.4234999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.739999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.2449999999999966E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7.2727272727272918E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B69-4BFB-BBBB-648CE9E06C16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395273728"/>
+        <c:axId val="395286208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="395273728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395286208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="395286208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395273728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5242,6 +5746,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7823,6 +8367,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8355,7 +9415,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8385,7 +9451,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8417,7 +9489,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8449,7 +9527,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8481,7 +9565,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8513,7 +9603,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8525,6 +9621,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31198619-082B-376B-1EAE-67D9768EF285}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8795,11 +9932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10448,23 +11585,443 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>5</v>
       </c>
-      <c r="B83" s="1">
-        <v>0</v>
-      </c>
-      <c r="C83" s="4">
+      <c r="B83" s="2">
+        <v>0</v>
+      </c>
+      <c r="C83" s="5">
         <v>39.996000000000002</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="7">
         <v>0.74060000000000004</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="7">
         <v>6.2899999999999998E-2</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="7">
         <v>-6.0699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>-4.9980000000000002</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" s="4">
+        <v>10</v>
+      </c>
+      <c r="D84" s="6">
+        <f>D2+0.0142</f>
+        <v>-0.13570000000000002</v>
+      </c>
+      <c r="E84" s="6">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="F84" s="6">
+        <v>-0.22070000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>-4</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" s="4">
+        <v>10</v>
+      </c>
+      <c r="D85" s="6">
+        <f t="shared" ref="D85:D103" si="0">D3+0.0142</f>
+        <v>-4.7600000000000003E-2</v>
+      </c>
+      <c r="E85" s="6">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="F85" s="6">
+        <v>-0.20319999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="4">
+        <v>10</v>
+      </c>
+      <c r="D86" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="E86" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F86" s="6">
+        <v>-0.1875</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" s="4">
+        <v>10</v>
+      </c>
+      <c r="D87" s="6">
+        <f t="shared" si="0"/>
+        <v>0.1331</v>
+      </c>
+      <c r="E87" s="6">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="F87" s="6">
+        <v>-0.1724</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0</v>
+      </c>
+      <c r="C88" s="4">
+        <v>10</v>
+      </c>
+      <c r="D88" s="6">
+        <f t="shared" si="0"/>
+        <v>0.2248</v>
+      </c>
+      <c r="E88" s="6">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="F88" s="6">
+        <v>-0.15959999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0</v>
+      </c>
+      <c r="C89" s="4">
+        <v>10</v>
+      </c>
+      <c r="D89" s="6">
+        <f t="shared" si="0"/>
+        <v>0.31779999999999997</v>
+      </c>
+      <c r="E89" s="6">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="F89" s="6">
+        <v>-0.1439</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>1</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0</v>
+      </c>
+      <c r="C90" s="4">
+        <v>10</v>
+      </c>
+      <c r="D90" s="6">
+        <f t="shared" si="0"/>
+        <v>0.40689999999999998</v>
+      </c>
+      <c r="E90" s="6">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="F90" s="6">
+        <v>-0.12939999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>2</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0</v>
+      </c>
+      <c r="C91" s="4">
+        <v>10</v>
+      </c>
+      <c r="D91" s="6">
+        <f t="shared" si="0"/>
+        <v>0.49869999999999998</v>
+      </c>
+      <c r="E91" s="6">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="F91" s="6">
+        <v>-0.1145</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>3</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0</v>
+      </c>
+      <c r="C92" s="4">
+        <v>10</v>
+      </c>
+      <c r="D92" s="6">
+        <f t="shared" si="0"/>
+        <v>0.58809999999999996</v>
+      </c>
+      <c r="E92" s="6">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="F92" s="6">
+        <v>-9.9500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>4</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0</v>
+      </c>
+      <c r="C93" s="4">
+        <v>10</v>
+      </c>
+      <c r="D93" s="6">
+        <f t="shared" si="0"/>
+        <v>0.6764</v>
+      </c>
+      <c r="E93" s="6">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F93" s="6">
+        <v>-8.3500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>5</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0</v>
+      </c>
+      <c r="C94" s="4">
+        <v>10</v>
+      </c>
+      <c r="D94" s="6">
+        <f t="shared" si="0"/>
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="E94" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F94" s="6">
+        <v>-6.8900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>6</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0</v>
+      </c>
+      <c r="C95" s="4">
+        <v>10</v>
+      </c>
+      <c r="D95" s="6">
+        <f t="shared" si="0"/>
+        <v>0.84540000000000004</v>
+      </c>
+      <c r="E95" s="6">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="F95" s="6">
+        <v>-5.3499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>7</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0</v>
+      </c>
+      <c r="C96" s="4">
+        <v>10</v>
+      </c>
+      <c r="D96" s="6">
+        <f t="shared" si="0"/>
+        <v>0.92230000000000001</v>
+      </c>
+      <c r="E96" s="6">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="F96" s="6">
+        <v>-3.7699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>8</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0</v>
+      </c>
+      <c r="C97" s="4">
+        <v>10</v>
+      </c>
+      <c r="D97" s="6">
+        <f t="shared" si="0"/>
+        <v>0.98309999999999997</v>
+      </c>
+      <c r="E97" s="6">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="F97" s="6">
+        <v>-2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>9</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" s="4">
+        <v>10</v>
+      </c>
+      <c r="D98" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0247999999999999</v>
+      </c>
+      <c r="E98" s="6">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="F98" s="6">
+        <v>-5.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>10</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0</v>
+      </c>
+      <c r="C99" s="4">
+        <v>10</v>
+      </c>
+      <c r="D99" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0547</v>
+      </c>
+      <c r="E99" s="6">
+        <v>0.1016</v>
+      </c>
+      <c r="F99" s="6">
+        <v>6.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>11</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0</v>
+      </c>
+      <c r="C100" s="4">
+        <v>10</v>
+      </c>
+      <c r="D100" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0681</v>
+      </c>
+      <c r="E100" s="6">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F100" s="6">
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0</v>
+      </c>
+      <c r="C101" s="4">
+        <v>10</v>
+      </c>
+      <c r="D101" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1087</v>
+      </c>
+      <c r="E101" s="6">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="F101" s="6">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>13</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0</v>
+      </c>
+      <c r="C102" s="4">
+        <v>10</v>
+      </c>
+      <c r="D102" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1218999999999999</v>
+      </c>
+      <c r="E102" s="6">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="F102" s="6">
+        <v>3.3E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>14</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0</v>
+      </c>
+      <c r="C103" s="4">
+        <v>10</v>
+      </c>
+      <c r="D103" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1689000000000001</v>
+      </c>
+      <c r="E103" s="7">
+        <v>0.17280000000000001</v>
+      </c>
+      <c r="F103" s="7">
+        <v>8.5000000000000006E-3</v>
       </c>
     </row>
   </sheetData>
@@ -10475,10 +12032,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -14710,4 +16267,1787 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F34B62-356D-42E1-A158-F1933CE34944}">
+  <dimension ref="A1:K83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>10</v>
+      </c>
+      <c r="I1" s="9">
+        <f>I2+K1</f>
+        <v>-1.4234999999999996E-2</v>
+      </c>
+      <c r="K1" s="9">
+        <f>I2-I3</f>
+        <v>-5.4949999999999999E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>-4.9980000000000002</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>19.992100000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <v>-0.14990000000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="F2" s="6">
+        <v>-0.22070000000000001</v>
+      </c>
+      <c r="G2" s="9">
+        <f>D22-D2</f>
+        <v>-2.0600000000000007E-2</v>
+      </c>
+      <c r="H2" s="6">
+        <v>20</v>
+      </c>
+      <c r="I2" s="9">
+        <f>AVERAGE(G2:G21)</f>
+        <v>-8.739999999999996E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>-4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>20.007200000000001</v>
+      </c>
+      <c r="D3" s="6">
+        <v>-6.1800000000000001E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>-0.20319999999999999</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G41" si="0">D23-D3</f>
+        <v>-1.77E-2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>30</v>
+      </c>
+      <c r="I3" s="9">
+        <f>AVERAGE(G22:G41)</f>
+        <v>-3.2449999999999966E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>20.001799999999999</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>-0.1875</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.5100000000000002E-2</v>
+      </c>
+      <c r="H4" s="6">
+        <v>40</v>
+      </c>
+      <c r="I4" s="9">
+        <f>AVERAGE(G42:G52)</f>
+        <v>-7.2727272727272918E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>19.998200000000001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.11890000000000001</v>
+      </c>
+      <c r="E5" s="6">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>-0.1724</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.1300000000000004E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>20.000499999999999</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.21060000000000001</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-0.15959999999999999</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.4000000000000186E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>20.001300000000001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.30359999999999998</v>
+      </c>
+      <c r="E7" s="6">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>-0.1439</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.8999999999999617E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>19.995100000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.39269999999999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>-0.12939999999999999</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.9000000000000137E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>19.999500000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.48449999999999999</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="F9" s="6">
+        <v>-0.1145</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.4000000000000132E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>20.004300000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.57389999999999997</v>
+      </c>
+      <c r="E10" s="6">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>-9.9500000000000005E-2</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.9999999999991189E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>20.000599999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-8.3500000000000005E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>19.996300000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.74939999999999996</v>
+      </c>
+      <c r="E12" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>-6.8900000000000003E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.6999999999999265E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>19.993300000000001</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.83120000000000005</v>
+      </c>
+      <c r="E13" s="6">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>-5.3499999999999999E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.4000000000000723E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>20.008600000000001</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.90810000000000002</v>
+      </c>
+      <c r="E14" s="6">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>-3.7699999999999997E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>20.008299999999998</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="E15" s="6">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="F15" s="6">
+        <v>-2.2499999999999999E-2</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.9000000000000199E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>19.993300000000001</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.0105999999999999</v>
+      </c>
+      <c r="E16" s="6">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>-5.1999999999999998E-3</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.5199999999999991E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>20.001300000000001</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1.0405</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.1016</v>
+      </c>
+      <c r="F17" s="6">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.71999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>20.001300000000001</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1.0539000000000001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.4499999999999957E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>19.991499999999998</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1.0945</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.9000000000000181E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>19.9802</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1.1076999999999999</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="F20" s="6">
+        <v>3.3E-3</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3900000000000032E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>19.990200000000002</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1.1547000000000001</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.17280000000000001</v>
+      </c>
+      <c r="F21" s="7">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.8000000000001375E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>-5</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>30.0017</v>
+      </c>
+      <c r="D22" s="6">
+        <v>-0.17050000000000001</v>
+      </c>
+      <c r="E22" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>-0.20649999999999999</v>
+      </c>
+      <c r="G22" s="9">
+        <f>D42-D22</f>
+        <v>-6.9999999999999785E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>-4.0019999999999998</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>29.991700000000002</v>
+      </c>
+      <c r="D23" s="6">
+        <v>-7.9500000000000001E-2</v>
+      </c>
+      <c r="E23" s="6">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>-0.19220000000000001</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.1999999999999963E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>-2.9980000000000002</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>29.995899999999999</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="E24" s="6">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="F24" s="6">
+        <v>-0.17860000000000001</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.4999999999999988E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>30.006</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.1076</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="F25" s="6">
+        <v>-0.16450000000000001</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000286E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>29.982700000000001</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.20219999999999999</v>
+      </c>
+      <c r="E26" s="6">
+        <v>4.9099999999999998E-2</v>
+      </c>
+      <c r="F26" s="6">
+        <v>-0.15079999999999999</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000066E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>29.994399999999999</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="F27" s="6">
+        <v>-0.13789999999999999</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999908E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>30.002199999999998</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="E28" s="6">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>-0.1237</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3000000000000242E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4">
+        <v>29.996099999999998</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.48209999999999997</v>
+      </c>
+      <c r="E29" s="6">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="F29" s="6">
+        <v>-0.10929999999999999</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000238E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="4">
+        <v>30.000599999999999</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.57310000000000005</v>
+      </c>
+      <c r="E30" s="6">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="F30" s="6">
+        <v>-9.4100000000000003E-2</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>29.9998</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.66020000000000001</v>
+      </c>
+      <c r="E31" s="6">
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="F31" s="6">
+        <v>-7.9100000000000004E-2</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.0000000000003393E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>29.995899999999999</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.74470000000000003</v>
+      </c>
+      <c r="E32" s="6">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="F32" s="6">
+        <v>-6.3600000000000004E-2</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0999999999999908E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>29.997800000000002</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.82479999999999998</v>
+      </c>
+      <c r="E33" s="6">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F33" s="6">
+        <v>-4.9399999999999999E-2</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.9000000000000146E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4">
+        <v>29.993600000000001</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="E34" s="6">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="F34" s="6">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.6000000000000485E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>29.995999999999999</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="E35" s="6">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="F35" s="6">
+        <v>-1.95E-2</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.7999999999999154E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>30.002199999999998</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="E36" s="6">
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="F36" s="6">
+        <v>-4.4999999999999997E-3</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.8299999999999983E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>10</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>29.9971</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1.0033000000000001</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.10539999999999999</v>
+      </c>
+      <c r="F37" s="6">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0800000000000032E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>11</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4">
+        <v>30.005299999999998</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1.0394000000000001</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.1181</v>
+      </c>
+      <c r="F38" s="6">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.2000000000002071E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4">
+        <v>30.0015</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.0866</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.13239999999999999</v>
+      </c>
+      <c r="F39" s="6">
+        <v>1.24E-2</v>
+      </c>
+      <c r="G39" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>13</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
+        <v>30.004300000000001</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.1315999999999999</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.14610000000000001</v>
+      </c>
+      <c r="F40" s="6">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="G40" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.3999999999998511E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>14</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="5">
+        <v>29.990200000000002</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1.1498999999999999</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="F41" s="7">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="G41" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3200000000000101E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>-4.9969999999999999</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4">
+        <v>39.996699999999997</v>
+      </c>
+      <c r="D42" s="6">
+        <v>-0.17749999999999999</v>
+      </c>
+      <c r="E42" s="6">
+        <v>4.9700000000000001E-2</v>
+      </c>
+      <c r="F42" s="6">
+        <v>-0.2016</v>
+      </c>
+      <c r="G42" s="9">
+        <f>D42-D62</f>
+        <v>2.2999999999999965E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>-4</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>40.007599999999996</v>
+      </c>
+      <c r="D43" s="6">
+        <v>-8.4699999999999998E-2</v>
+      </c>
+      <c r="E43" s="6">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="F43" s="6">
+        <v>-0.1888</v>
+      </c>
+      <c r="G43" s="9">
+        <f t="shared" ref="G43:G51" si="1">D43-D63</f>
+        <v>3.9999999999999758E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>40.0017</v>
+      </c>
+      <c r="D44" s="6">
+        <v>1.14E-2</v>
+      </c>
+      <c r="E44" s="6">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="F44" s="6">
+        <v>-0.17560000000000001</v>
+      </c>
+      <c r="G44" s="9">
+        <f t="shared" si="1"/>
+        <v>-5.0000000000000044E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>40.008099999999999</v>
+      </c>
+      <c r="D45" s="6">
+        <v>0.1075</v>
+      </c>
+      <c r="E45" s="6">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="F45" s="6">
+        <v>-0.16220000000000001</v>
+      </c>
+      <c r="G45" s="9">
+        <f t="shared" si="1"/>
+        <v>-1.2999999999999956E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>40</v>
+      </c>
+      <c r="D46" s="6">
+        <v>0.2034</v>
+      </c>
+      <c r="E46" s="6">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="F46" s="6">
+        <v>-0.14860000000000001</v>
+      </c>
+      <c r="G46" s="9">
+        <f t="shared" si="1"/>
+        <v>-1.4000000000000123E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
+        <v>39.9893</v>
+      </c>
+      <c r="D47" s="6">
+        <v>0.29880000000000001</v>
+      </c>
+      <c r="E47" s="6">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="F47" s="6">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="G47" s="9">
+        <f t="shared" si="1"/>
+        <v>-9.000000000000119E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
+        <v>40.000999999999998</v>
+      </c>
+      <c r="D48" s="6">
+        <v>0.3921</v>
+      </c>
+      <c r="E48" s="6">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="F48" s="6">
+        <v>-0.12089999999999999</v>
+      </c>
+      <c r="G48" s="9">
+        <f t="shared" si="1"/>
+        <v>-6.9999999999997842E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>2</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <v>40.007100000000001</v>
+      </c>
+      <c r="D49" s="6">
+        <v>0.4839</v>
+      </c>
+      <c r="E49" s="6">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F49" s="6">
+        <v>-0.10639999999999999</v>
+      </c>
+      <c r="G49" s="9">
+        <f t="shared" si="1"/>
+        <v>-8.0000000000002292E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>3</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
+        <v>39.994900000000001</v>
+      </c>
+      <c r="D50" s="6">
+        <v>0.57320000000000004</v>
+      </c>
+      <c r="E50" s="6">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="F50" s="6">
+        <v>-9.1399999999999995E-2</v>
+      </c>
+      <c r="G50" s="9">
+        <f t="shared" si="1"/>
+        <v>-1.1999999999999789E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4">
+        <v>39.996600000000001</v>
+      </c>
+      <c r="D51" s="6">
+        <v>0.65949999999999998</v>
+      </c>
+      <c r="E51" s="6">
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="F51" s="6">
+        <v>-7.6100000000000001E-2</v>
+      </c>
+      <c r="G51" s="9">
+        <f>D51-D71</f>
+        <v>-1.6000000000000458E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4">
+        <v>39.9878</v>
+      </c>
+      <c r="D52" s="6">
+        <v>0.74260000000000004</v>
+      </c>
+      <c r="E52" s="6">
+        <v>6.2600000000000003E-2</v>
+      </c>
+      <c r="F52" s="6">
+        <v>-6.0699999999999997E-2</v>
+      </c>
+      <c r="G52" s="9">
+        <f>D52-D72</f>
+        <v>-2.2999999999999687E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>6</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" s="4">
+        <v>40.0017</v>
+      </c>
+      <c r="D53" s="6">
+        <v>0.82089999999999996</v>
+      </c>
+      <c r="E53" s="6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F53" s="6">
+        <v>-4.5600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>7</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="4">
+        <v>39.994199999999999</v>
+      </c>
+      <c r="D54" s="6">
+        <v>0.89349999999999996</v>
+      </c>
+      <c r="E54" s="6">
+        <v>7.2300000000000003E-2</v>
+      </c>
+      <c r="F54" s="6">
+        <v>-3.09E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" s="4">
+        <v>39.994</v>
+      </c>
+      <c r="D55" s="6">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="E55" s="6">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="F55" s="6">
+        <v>-1.6899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>9</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="4">
+        <v>39.990600000000001</v>
+      </c>
+      <c r="D56" s="6">
+        <v>0.97709999999999997</v>
+      </c>
+      <c r="E56" s="6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F56" s="6">
+        <v>-7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>10</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4">
+        <v>39.994900000000001</v>
+      </c>
+      <c r="D57" s="6">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0.1067</v>
+      </c>
+      <c r="F57" s="6">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>11</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="4">
+        <v>39.996000000000002</v>
+      </c>
+      <c r="D58" s="6">
+        <v>1.0311999999999999</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0.1183</v>
+      </c>
+      <c r="F58" s="6">
+        <v>8.3999999999999995E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>12</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4">
+        <v>40.002000000000002</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1.0766</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0.13089999999999999</v>
+      </c>
+      <c r="F59" s="6">
+        <v>1.41E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>13</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="4">
+        <v>39.993299999999998</v>
+      </c>
+      <c r="D60" s="6">
+        <v>1.1242000000000001</v>
+      </c>
+      <c r="E60" s="6">
+        <v>0.1457</v>
+      </c>
+      <c r="F60" s="6">
+        <v>1.83E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>14</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0</v>
+      </c>
+      <c r="C61" s="5">
+        <v>39.999499999999998</v>
+      </c>
+      <c r="D61" s="7">
+        <v>1.1631</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="F61" s="7">
+        <v>2.47E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>-5</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4">
+        <v>49.992699999999999</v>
+      </c>
+      <c r="D62" s="6">
+        <v>-0.17979999999999999</v>
+      </c>
+      <c r="E62" s="6">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="F62" s="6">
+        <v>-0.20069999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>-4</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="4">
+        <v>49.990499999999997</v>
+      </c>
+      <c r="D63" s="6">
+        <v>-8.5099999999999995E-2</v>
+      </c>
+      <c r="E63" s="6">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="F63" s="6">
+        <v>-0.18779999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="4">
+        <v>49.995100000000001</v>
+      </c>
+      <c r="D64" s="6">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="E64" s="6">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="F64" s="6">
+        <v>-0.17460000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" s="4">
+        <v>49.992100000000001</v>
+      </c>
+      <c r="D65" s="6">
+        <v>0.10879999999999999</v>
+      </c>
+      <c r="E65" s="6">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="F65" s="6">
+        <v>-0.161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="4">
+        <v>49.985199999999999</v>
+      </c>
+      <c r="D66" s="6">
+        <v>0.20480000000000001</v>
+      </c>
+      <c r="E66" s="6">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="F66" s="6">
+        <v>-0.14760000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="4">
+        <v>49.9846</v>
+      </c>
+      <c r="D67" s="6">
+        <v>0.29970000000000002</v>
+      </c>
+      <c r="E67" s="6">
+        <v>4.6699999999999998E-2</v>
+      </c>
+      <c r="F67" s="6">
+        <v>-0.1338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>1</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="4">
+        <v>49.990099999999998</v>
+      </c>
+      <c r="D68" s="6">
+        <v>0.39279999999999998</v>
+      </c>
+      <c r="E68" s="6">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="F68" s="6">
+        <v>-0.1193</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>2</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" s="4">
+        <v>50.002499999999998</v>
+      </c>
+      <c r="D69" s="6">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="E69" s="6">
+        <v>5.0599999999999999E-2</v>
+      </c>
+      <c r="F69" s="6">
+        <v>-0.1043</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>3</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="4">
+        <v>49.999499999999998</v>
+      </c>
+      <c r="D70" s="6">
+        <v>0.57440000000000002</v>
+      </c>
+      <c r="E70" s="6">
+        <v>5.33E-2</v>
+      </c>
+      <c r="F70" s="6">
+        <v>-8.8900000000000007E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>4</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="4">
+        <v>49.993200000000002</v>
+      </c>
+      <c r="D71" s="6">
+        <v>0.66110000000000002</v>
+      </c>
+      <c r="E71" s="6">
+        <v>5.6500000000000002E-2</v>
+      </c>
+      <c r="F71" s="6">
+        <v>-7.3700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>5</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0</v>
+      </c>
+      <c r="C72" s="5">
+        <v>50.018000000000001</v>
+      </c>
+      <c r="D72" s="7">
+        <v>0.74490000000000001</v>
+      </c>
+      <c r="E72" s="7">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="F72" s="7">
+        <v>-5.8799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>